<commit_message>
Realização de tarefas do Jira
</commit_message>
<xml_diff>
--- a/Editables/Relação dos Conceitos.xlsx
+++ b/Editables/Relação dos Conceitos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uapt33090-my.sharepoint.com/personal/t_fonseca_ua_pt/Documents/Desktop/Tiago/2 Ano/AS/AS/Projeto/Fase-2/Editables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="260" documentId="8_{44642A0E-22BE-4ED1-97DF-D65E5D85DA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68DDF646-24E9-4ED9-928C-96545043C141}"/>
+  <xr:revisionPtr revIDLastSave="267" documentId="8_{44642A0E-22BE-4ED1-97DF-D65E5D85DA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D86AA6F3-780B-43C1-91D0-7BF01F1507E9}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16200" activeTab="1" xr2:uid="{9379EE56-B285-449C-84DD-477034C971AA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{9379EE56-B285-449C-84DD-477034C971AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha2" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>Cliente</t>
   </si>
@@ -97,6 +97,9 @@
   <si>
     <t>Realizar
 Operações</t>
+  </si>
+  <si>
+    <t>Recuperar Password</t>
   </si>
 </sst>
 </file>
@@ -263,19 +266,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -287,19 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -634,10 +637,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B5DF4A-9943-4A3A-8571-26C59D92923E}">
-  <dimension ref="C10:H28"/>
+  <dimension ref="C10:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,213 +650,235 @@
   <sheetData>
     <row r="10" spans="3:8" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="H11" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="14"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4" t="s">
+      <c r="G13" s="6"/>
+      <c r="H13" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="3"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4" t="s">
+      <c r="G15" s="6"/>
+      <c r="H15" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="3"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4" t="s">
+      <c r="G17" s="6"/>
+      <c r="H17" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="3"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="3"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4" t="s">
+      <c r="G21" s="6"/>
+      <c r="H21" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="3"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6" t="s">
+      <c r="F23" s="14"/>
+      <c r="G23" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H23" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="3"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4" t="s">
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="4"/>
+      <c r="H25" s="6"/>
     </row>
     <row r="26" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="3"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4" t="s">
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="4"/>
+      <c r="H27" s="6"/>
     </row>
     <row r="28" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="3"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D29" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="5"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D11:D12"/>
+  <mergeCells count="50">
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:G20"/>
@@ -862,6 +887,12 @@
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="H21:H22"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D20"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="G15:G16"/>
@@ -869,19 +900,18 @@
     <mergeCell ref="E17:E18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>